<commit_message>
EPS: add diode and grounded holes. OBC: a lot of changes
</commit_message>
<xml_diff>
--- a/SubSystems/Electrical Power System/Hardware/EPS_V1/Project Outputs for EPS_V1/3D_and_pcb/BOM/BOM_JLC.xlsx
+++ b/SubSystems/Electrical Power System/Hardware/EPS_V1/Project Outputs for EPS_V1/3D_and_pcb/BOM/BOM_JLC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!MEGA\!myFiles\ArianSat-Stratosphere\SubSystems\Electrical Power System\Hardware\EPS_V1\Project Outputs for EPS_V1\3D_and_pcb\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62ED41C-AB1F-4A29-BA52-BC2094491366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FDE67EC-8B36-4713-BBFC-92080B907C35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{25D651B7-B704-4539-A279-A1B32B854629}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="234">
   <si>
     <t>Comment</t>
   </si>
@@ -142,12 +142,6 @@
   </si>
   <si>
     <t/>
-  </si>
-  <si>
-    <t>Additional order1, Additional order2, Additional order3, Additional order4, C85, FLT1</t>
-  </si>
-  <si>
-    <t>[NoValue], DCS5R5224H, IND 0603</t>
   </si>
   <si>
     <t>!Generic P MOSFET</t>
@@ -1189,10 +1183,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{528F7681-1332-45C3-B7F8-CEF0B1B43AB9}">
-  <dimension ref="A1:S98"/>
+  <dimension ref="A1:S97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1215,7 +1209,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E1" s="9"/>
       <c r="F1" s="10"/>
@@ -1244,7 +1238,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="10"/>
@@ -1273,7 +1267,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="10"/>
@@ -1302,7 +1296,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="10"/>
@@ -1331,7 +1325,7 @@
         <v>14</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="10"/>
@@ -1360,7 +1354,7 @@
         <v>17</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="10"/>
@@ -1389,7 +1383,7 @@
         <v>20</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="10"/>
@@ -1418,7 +1412,7 @@
         <v>23</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="10"/>
@@ -1447,7 +1441,7 @@
         <v>20</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="10"/>
@@ -1476,7 +1470,7 @@
         <v>28</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="10"/>
@@ -1505,7 +1499,7 @@
         <v>31</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="10"/>
@@ -1534,7 +1528,7 @@
         <v>34</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="10"/>
@@ -1563,7 +1557,7 @@
         <v>35</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="10"/>
@@ -1583,17 +1577,15 @@
     </row>
     <row r="14" spans="1:19">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>196</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D14" s="5"/>
       <c r="E14" s="11"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
@@ -1612,15 +1604,17 @@
     </row>
     <row r="15" spans="1:19">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="5"/>
+        <v>43</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>200</v>
+      </c>
       <c r="E15" s="11"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
@@ -1639,16 +1633,16 @@
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="E16" s="11"/>
       <c r="F16" s="10"/>
@@ -1666,81 +1660,67 @@
       <c r="R16" s="10"/>
       <c r="S16" s="10"/>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="10"/>
-      <c r="R17" s="10"/>
-      <c r="S17" s="10"/>
-    </row>
-    <row r="18" spans="1:19">
+        <v>194</v>
+      </c>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="D20" s="5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E20" s="8"/>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
         <v>58</v>
       </c>
@@ -1748,14 +1728,12 @@
         <v>59</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>203</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="D21" s="5"/>
       <c r="E21" s="8"/>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
         <v>60</v>
       </c>
@@ -1763,42 +1741,44 @@
         <v>61</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="5"/>
+        <v>62</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>37</v>
+        <v>65</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>219</v>
       </c>
       <c r="E23" s="8"/>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>221</v>
+      <c r="D24" s="5" t="s">
+        <v>203</v>
       </c>
       <c r="E24" s="8"/>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
         <v>68</v>
       </c>
@@ -1806,14 +1786,14 @@
         <v>69</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="E25" s="8"/>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
         <v>70</v>
       </c>
@@ -1821,14 +1801,14 @@
         <v>71</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
         <v>72</v>
       </c>
@@ -1836,14 +1816,14 @@
         <v>73</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:5">
       <c r="A28" s="1" t="s">
         <v>74</v>
       </c>
@@ -1851,14 +1831,14 @@
         <v>75</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E28" s="8"/>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
         <v>76</v>
       </c>
@@ -1866,14 +1846,14 @@
         <v>77</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>214</v>
+        <v>65</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>218</v>
       </c>
       <c r="E29" s="8"/>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
         <v>78</v>
       </c>
@@ -1881,29 +1861,29 @@
         <v>79</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>220</v>
+        <v>80</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>213</v>
       </c>
       <c r="E30" s="8"/>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:5">
       <c r="A31" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="D31" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E31" s="8"/>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
         <v>83</v>
       </c>
@@ -1911,10 +1891,10 @@
         <v>84</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="E32" s="8"/>
     </row>
@@ -1926,10 +1906,10 @@
         <v>86</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E33" s="8"/>
     </row>
@@ -1941,10 +1921,10 @@
         <v>88</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E34" s="8"/>
     </row>
@@ -1953,85 +1933,83 @@
         <v>89</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>90</v>
+        <v>216</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="E35" s="8"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>218</v>
-      </c>
       <c r="C36" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>217</v>
+        <v>92</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>194</v>
       </c>
       <c r="E36" s="8"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>196</v>
+        <v>95</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>194</v>
       </c>
       <c r="E37" s="8"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" ht="15.75">
       <c r="A38" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>196</v>
+        <v>98</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>217</v>
       </c>
       <c r="E38" s="8"/>
     </row>
-    <row r="39" spans="1:5" ht="15.75">
+    <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D39" s="13" t="s">
-        <v>219</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="D39" s="5"/>
       <c r="E39" s="8"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="8"/>
@@ -2044,20 +2022,20 @@
         <v>105</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>108</v>
+        <v>40</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="8"/>
@@ -2070,53 +2048,55 @@
         <v>110</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D43" s="5"/>
+        <v>111</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>194</v>
+      </c>
       <c r="E43" s="8"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E44" s="8"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="E45" s="8"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="D46" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E46" s="8"/>
     </row>
@@ -2128,11 +2108,9 @@
         <v>121</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>207</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="D47" s="5"/>
       <c r="E47" s="8"/>
     </row>
     <row r="48" spans="1:5">
@@ -2143,7 +2121,7 @@
         <v>123</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="8"/>
@@ -2156,9 +2134,11 @@
         <v>125</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D49" s="5"/>
+        <v>117</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>206</v>
+      </c>
       <c r="E49" s="8"/>
     </row>
     <row r="50" spans="1:5">
@@ -2169,11 +2149,9 @@
         <v>127</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>208</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="D50" s="5"/>
       <c r="E50" s="8"/>
     </row>
     <row r="51" spans="1:5">
@@ -2184,7 +2162,7 @@
         <v>129</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="8"/>
@@ -2197,7 +2175,7 @@
         <v>131</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="8"/>
@@ -2210,9 +2188,11 @@
         <v>133</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D53" s="5"/>
+        <v>117</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>223</v>
+      </c>
       <c r="E53" s="8"/>
     </row>
     <row r="54" spans="1:5">
@@ -2223,11 +2203,9 @@
         <v>135</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>225</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="D54" s="5"/>
       <c r="E54" s="8"/>
     </row>
     <row r="55" spans="1:5">
@@ -2238,9 +2216,11 @@
         <v>137</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D55" s="5"/>
+        <v>117</v>
+      </c>
+      <c r="D55" s="14" t="s">
+        <v>222</v>
+      </c>
       <c r="E55" s="8"/>
     </row>
     <row r="56" spans="1:5">
@@ -2251,10 +2231,10 @@
         <v>139</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D56" s="14" t="s">
-        <v>224</v>
+        <v>117</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>222</v>
       </c>
       <c r="E56" s="8"/>
     </row>
@@ -2266,11 +2246,9 @@
         <v>141</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>224</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="D57" s="5"/>
       <c r="E57" s="8"/>
     </row>
     <row r="58" spans="1:5">
@@ -2281,7 +2259,7 @@
         <v>143</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="8"/>
@@ -2294,9 +2272,11 @@
         <v>145</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D59" s="5"/>
+        <v>117</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>229</v>
+      </c>
       <c r="E59" s="8"/>
     </row>
     <row r="60" spans="1:5">
@@ -2307,10 +2287,10 @@
         <v>147</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="E60" s="8"/>
     </row>
@@ -2322,11 +2302,9 @@
         <v>149</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>223</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="D61" s="5"/>
       <c r="E61" s="8"/>
     </row>
     <row r="62" spans="1:5">
@@ -2337,9 +2315,11 @@
         <v>151</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D62" s="5"/>
+        <v>117</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>220</v>
+      </c>
       <c r="E62" s="8"/>
     </row>
     <row r="63" spans="1:5">
@@ -2350,11 +2330,9 @@
         <v>153</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>222</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="D63" s="5"/>
       <c r="E63" s="8"/>
     </row>
     <row r="64" spans="1:5">
@@ -2365,7 +2343,7 @@
         <v>155</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="8"/>
@@ -2378,7 +2356,7 @@
         <v>157</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="8"/>
@@ -2391,9 +2369,11 @@
         <v>159</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D66" s="5"/>
+        <v>117</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>228</v>
+      </c>
       <c r="E66" s="8"/>
     </row>
     <row r="67" spans="1:5">
@@ -2404,10 +2384,10 @@
         <v>161</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E67" s="8"/>
     </row>
@@ -2419,11 +2399,9 @@
         <v>163</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>229</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="D68" s="5"/>
       <c r="E68" s="8"/>
     </row>
     <row r="69" spans="1:5">
@@ -2434,9 +2412,11 @@
         <v>165</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D69" s="5"/>
+        <v>117</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>226</v>
+      </c>
       <c r="E69" s="8"/>
     </row>
     <row r="70" spans="1:5">
@@ -2447,11 +2427,9 @@
         <v>167</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>228</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="D70" s="5"/>
       <c r="E70" s="8"/>
     </row>
     <row r="71" spans="1:5">
@@ -2462,7 +2440,7 @@
         <v>169</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D71" s="5"/>
       <c r="E71" s="8"/>
@@ -2475,24 +2453,24 @@
         <v>171</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D72" s="5"/>
+        <v>172</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>224</v>
+      </c>
       <c r="E72" s="8"/>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>226</v>
-      </c>
+      <c r="D73" s="5"/>
       <c r="E73" s="8"/>
     </row>
     <row r="74" spans="1:5">
@@ -2503,7 +2481,7 @@
         <v>176</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D74" s="5"/>
       <c r="E74" s="8"/>
@@ -2516,35 +2494,35 @@
         <v>178</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D75" s="5"/>
+        <v>179</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>225</v>
+      </c>
       <c r="E75" s="8"/>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>227</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="D76" s="5"/>
       <c r="E76" s="8"/>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C77" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>184</v>
       </c>
       <c r="D77" s="5"/>
       <c r="E77" s="8"/>
@@ -2557,106 +2535,93 @@
         <v>186</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D78" s="5"/>
+        <v>187</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>231</v>
+      </c>
       <c r="E78" s="8"/>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E79" s="8"/>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C80" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B80" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>192</v>
-      </c>
       <c r="D80" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E80" s="8"/>
     </row>
-    <row r="81" spans="1:5">
-      <c r="A81" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D81" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="E81" s="8"/>
-    </row>
-    <row r="82" spans="1:5">
+    <row r="81" spans="5:5">
+      <c r="E81" s="7"/>
+    </row>
+    <row r="82" spans="5:5">
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="5:5">
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="5:5">
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="5:5">
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="5:5">
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="5:5">
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="5:5">
       <c r="E88" s="7"/>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="5:5">
       <c r="E89" s="7"/>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="5:5">
       <c r="E90" s="7"/>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="5:5">
       <c r="E91" s="7"/>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="5:5">
       <c r="E92" s="7"/>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="5:5">
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="5:5">
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="5:5">
       <c r="E95" s="7"/>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="5:5">
       <c r="E96" s="7"/>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="7"/>
-    </row>
-    <row r="98" spans="5:5">
-      <c r="E98" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
EPS SMT final version
</commit_message>
<xml_diff>
--- a/SubSystems/Electrical Power System/Hardware/EPS_V1/Project Outputs for EPS_V1/3D_and_pcb/BOM/BOM_JLC.xlsx
+++ b/SubSystems/Electrical Power System/Hardware/EPS_V1/Project Outputs for EPS_V1/3D_and_pcb/BOM/BOM_JLC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!MEGA\!myFiles\ArianSat-Stratosphere\SubSystems\Electrical Power System\Hardware\EPS_V1\Project Outputs for EPS_V1\3D_and_pcb\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FDE67EC-8B36-4713-BBFC-92080B907C35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9A13FE-F48C-4D46-B99B-A0B1122697AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{25D651B7-B704-4539-A279-A1B32B854629}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="241">
   <si>
     <t>Comment</t>
   </si>
@@ -730,13 +730,34 @@
   </si>
   <si>
     <t>C7220</t>
+  </si>
+  <si>
+    <t>LED 0603 Red</t>
+  </si>
+  <si>
+    <t>LED1</t>
+  </si>
+  <si>
+    <t>LED 0603</t>
+  </si>
+  <si>
+    <t>RES 0402 1M</t>
+  </si>
+  <si>
+    <t>R128, R129, R130, R131</t>
+  </si>
+  <si>
+    <t>C26083</t>
+  </si>
+  <si>
+    <t>C84256</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -767,15 +788,6 @@
       <charset val="204"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
@@ -803,7 +815,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -826,50 +838,32 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Гиперссылка" xfId="2" builtinId="8"/>
+  <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1" xr:uid="{ECC4AF2B-832D-4EF0-9F9B-10CA043E980F}"/>
   </cellStyles>
@@ -1185,8 +1179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{528F7681-1332-45C3-B7F8-CEF0B1B43AB9}">
   <dimension ref="A1:S97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1196,6 +1190,7 @@
     <col min="3" max="3" width="32.7109375" customWidth="1"/>
     <col min="4" max="4" width="22.28515625" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15.75">
@@ -1208,24 +1203,24 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="1" t="s">
@@ -1237,24 +1232,24 @@
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" s="1" t="s">
@@ -1266,24 +1261,24 @@
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="1" t="s">
@@ -1295,24 +1290,24 @@
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="1" t="s">
@@ -1324,24 +1319,24 @@
       <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="1" t="s">
@@ -1353,24 +1348,24 @@
       <c r="C6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="1" t="s">
@@ -1382,24 +1377,24 @@
       <c r="C7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10"/>
-      <c r="S7" s="10"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="1" t="s">
@@ -1411,24 +1406,24 @@
       <c r="C8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="10"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="1" t="s">
@@ -1440,24 +1435,24 @@
       <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
-      <c r="S9" s="10"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="1" t="s">
@@ -1469,24 +1464,24 @@
       <c r="C10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="10"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="1" t="s">
@@ -1498,24 +1493,24 @@
       <c r="C11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="10"/>
-      <c r="S11" s="10"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="1" t="s">
@@ -1527,24 +1522,24 @@
       <c r="C12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="10"/>
-      <c r="S12" s="10"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="1" t="s">
@@ -1556,24 +1551,24 @@
       <c r="C13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="10"/>
-      <c r="S13" s="10"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
     </row>
     <row r="14" spans="1:19">
       <c r="A14" s="1" t="s">
@@ -1585,22 +1580,22 @@
       <c r="C14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="10"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
     </row>
     <row r="15" spans="1:19">
       <c r="A15" s="1" t="s">
@@ -1612,24 +1607,24 @@
       <c r="C15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="10"/>
-      <c r="S15" s="10"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="1" t="s">
@@ -1641,26 +1636,26 @@
       <c r="C16" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10"/>
-      <c r="S16" s="10"/>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
         <v>47</v>
       </c>
@@ -1670,12 +1665,15 @@
       <c r="C17" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="E17" s="8"/>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
         <v>50</v>
       </c>
@@ -1685,12 +1683,15 @@
       <c r="C18" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="E18" s="8"/>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
         <v>53</v>
       </c>
@@ -1700,12 +1701,15 @@
       <c r="C19" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="E19" s="8"/>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
         <v>56</v>
       </c>
@@ -1715,12 +1719,15 @@
       <c r="C20" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="E20" s="8"/>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
         <v>58</v>
       </c>
@@ -1730,10 +1737,13 @@
       <c r="C21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="8"/>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="D21" s="9"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
         <v>60</v>
       </c>
@@ -1743,12 +1753,15 @@
       <c r="C22" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="8"/>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
         <v>63</v>
       </c>
@@ -1758,12 +1771,15 @@
       <c r="C23" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="E23" s="8"/>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
         <v>66</v>
       </c>
@@ -1773,12 +1789,15 @@
       <c r="C24" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="E24" s="8"/>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
         <v>68</v>
       </c>
@@ -1788,12 +1807,15 @@
       <c r="C25" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="E25" s="8"/>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
         <v>70</v>
       </c>
@@ -1803,12 +1825,15 @@
       <c r="C26" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="E26" s="8"/>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
         <v>72</v>
       </c>
@@ -1818,12 +1843,15 @@
       <c r="C27" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="E27" s="8"/>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
         <v>74</v>
       </c>
@@ -1833,12 +1861,15 @@
       <c r="C28" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="E28" s="8"/>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
         <v>76</v>
       </c>
@@ -1848,12 +1879,15 @@
       <c r="C29" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="E29" s="8"/>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
         <v>78</v>
       </c>
@@ -1863,12 +1897,15 @@
       <c r="C30" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="E30" s="8"/>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
         <v>81</v>
       </c>
@@ -1878,12 +1915,15 @@
       <c r="C31" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="E31" s="8"/>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="4"/>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
         <v>83</v>
       </c>
@@ -1893,12 +1933,15 @@
       <c r="C32" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="E32" s="8"/>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
         <v>85</v>
       </c>
@@ -1908,12 +1951,15 @@
       <c r="C33" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="E33" s="8"/>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="4"/>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
         <v>87</v>
       </c>
@@ -1923,12 +1969,15 @@
       <c r="C34" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="E34" s="8"/>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="4"/>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
         <v>89</v>
       </c>
@@ -1938,12 +1987,15 @@
       <c r="C35" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="E35" s="8"/>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="4"/>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
         <v>90</v>
       </c>
@@ -1953,12 +2005,15 @@
       <c r="C36" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="E36" s="8"/>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
         <v>93</v>
       </c>
@@ -1968,12 +2023,15 @@
       <c r="C37" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="E37" s="8"/>
-    </row>
-    <row r="38" spans="1:5" ht="15.75">
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="1:8" ht="15.75">
       <c r="A38" s="1" t="s">
         <v>96</v>
       </c>
@@ -1983,12 +2041,15 @@
       <c r="C38" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D38" s="13" t="s">
+      <c r="D38" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="E38" s="8"/>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
         <v>99</v>
       </c>
@@ -1998,10 +2059,13 @@
       <c r="C39" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D39" s="5"/>
-      <c r="E39" s="8"/>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="D39" s="9"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
         <v>102</v>
       </c>
@@ -2011,10 +2075,13 @@
       <c r="C40" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D40" s="5"/>
-      <c r="E40" s="8"/>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="D40" s="9"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
         <v>104</v>
       </c>
@@ -2024,10 +2091,13 @@
       <c r="C41" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D41" s="5"/>
-      <c r="E41" s="8"/>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="D41" s="9"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
         <v>107</v>
       </c>
@@ -2037,10 +2107,13 @@
       <c r="C42" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D42" s="5"/>
-      <c r="E42" s="8"/>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="D42" s="9"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
         <v>109</v>
       </c>
@@ -2050,12 +2123,15 @@
       <c r="C43" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D43" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="E43" s="8"/>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
         <v>112</v>
       </c>
@@ -2065,12 +2141,15 @@
       <c r="C44" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D44" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="E44" s="8"/>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="4"/>
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
         <v>115</v>
       </c>
@@ -2080,12 +2159,15 @@
       <c r="C45" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="E45" s="8"/>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
         <v>118</v>
       </c>
@@ -2095,12 +2177,15 @@
       <c r="C46" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="E46" s="8"/>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="4"/>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
         <v>120</v>
       </c>
@@ -2110,10 +2195,13 @@
       <c r="C47" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D47" s="5"/>
-      <c r="E47" s="8"/>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="D47" s="9"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="4"/>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
         <v>122</v>
       </c>
@@ -2123,10 +2211,13 @@
       <c r="C48" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D48" s="5"/>
-      <c r="E48" s="8"/>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="D48" s="9"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="4"/>
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49" s="1" t="s">
         <v>124</v>
       </c>
@@ -2136,12 +2227,15 @@
       <c r="C49" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D49" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="E49" s="8"/>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="4"/>
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50" s="1" t="s">
         <v>126</v>
       </c>
@@ -2151,10 +2245,13 @@
       <c r="C50" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D50" s="5"/>
-      <c r="E50" s="8"/>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="D50" s="9"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="4"/>
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
         <v>128</v>
       </c>
@@ -2164,10 +2261,13 @@
       <c r="C51" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D51" s="5"/>
-      <c r="E51" s="8"/>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="D51" s="9"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="4"/>
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52" s="1" t="s">
         <v>130</v>
       </c>
@@ -2177,10 +2277,13 @@
       <c r="C52" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D52" s="5"/>
-      <c r="E52" s="8"/>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="D52" s="9"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="1:8">
       <c r="A53" s="1" t="s">
         <v>132</v>
       </c>
@@ -2190,12 +2293,15 @@
       <c r="C53" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="D53" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="E53" s="8"/>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="4"/>
+    </row>
+    <row r="54" spans="1:8">
       <c r="A54" s="1" t="s">
         <v>134</v>
       </c>
@@ -2205,10 +2311,13 @@
       <c r="C54" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D54" s="5"/>
-      <c r="E54" s="8"/>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="D54" s="9"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="4"/>
+    </row>
+    <row r="55" spans="1:8">
       <c r="A55" s="1" t="s">
         <v>136</v>
       </c>
@@ -2218,12 +2327,15 @@
       <c r="C55" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D55" s="14" t="s">
+      <c r="D55" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="E55" s="8"/>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="4"/>
+    </row>
+    <row r="56" spans="1:8">
       <c r="A56" s="1" t="s">
         <v>138</v>
       </c>
@@ -2233,12 +2345,15 @@
       <c r="C56" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="D56" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="E56" s="8"/>
-    </row>
-    <row r="57" spans="1:5">
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="4"/>
+    </row>
+    <row r="57" spans="1:8">
       <c r="A57" s="1" t="s">
         <v>140</v>
       </c>
@@ -2248,10 +2363,13 @@
       <c r="C57" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D57" s="5"/>
-      <c r="E57" s="8"/>
-    </row>
-    <row r="58" spans="1:5">
+      <c r="D57" s="9"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="4"/>
+    </row>
+    <row r="58" spans="1:8">
       <c r="A58" s="1" t="s">
         <v>142</v>
       </c>
@@ -2261,10 +2379,13 @@
       <c r="C58" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D58" s="5"/>
-      <c r="E58" s="8"/>
-    </row>
-    <row r="59" spans="1:5">
+      <c r="D58" s="9"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="4"/>
+    </row>
+    <row r="59" spans="1:8">
       <c r="A59" s="1" t="s">
         <v>144</v>
       </c>
@@ -2274,12 +2395,15 @@
       <c r="C59" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="D59" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="E59" s="8"/>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="4"/>
+    </row>
+    <row r="60" spans="1:8">
       <c r="A60" s="1" t="s">
         <v>146</v>
       </c>
@@ -2289,12 +2413,15 @@
       <c r="C60" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="D60" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="E60" s="8"/>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="4"/>
+    </row>
+    <row r="61" spans="1:8">
       <c r="A61" s="1" t="s">
         <v>148</v>
       </c>
@@ -2304,10 +2431,13 @@
       <c r="C61" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D61" s="5"/>
-      <c r="E61" s="8"/>
-    </row>
-    <row r="62" spans="1:5">
+      <c r="D61" s="9"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="4"/>
+    </row>
+    <row r="62" spans="1:8">
       <c r="A62" s="1" t="s">
         <v>150</v>
       </c>
@@ -2317,12 +2447,15 @@
       <c r="C62" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D62" s="5" t="s">
+      <c r="D62" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="E62" s="8"/>
-    </row>
-    <row r="63" spans="1:5">
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="4"/>
+    </row>
+    <row r="63" spans="1:8">
       <c r="A63" s="1" t="s">
         <v>152</v>
       </c>
@@ -2332,10 +2465,13 @@
       <c r="C63" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D63" s="5"/>
-      <c r="E63" s="8"/>
-    </row>
-    <row r="64" spans="1:5">
+      <c r="D63" s="9"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="4"/>
+    </row>
+    <row r="64" spans="1:8">
       <c r="A64" s="1" t="s">
         <v>154</v>
       </c>
@@ -2345,10 +2481,13 @@
       <c r="C64" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D64" s="5"/>
-      <c r="E64" s="8"/>
-    </row>
-    <row r="65" spans="1:5">
+      <c r="D64" s="9"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="4"/>
+    </row>
+    <row r="65" spans="1:8">
       <c r="A65" s="1" t="s">
         <v>156</v>
       </c>
@@ -2358,10 +2497,13 @@
       <c r="C65" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D65" s="5"/>
-      <c r="E65" s="8"/>
-    </row>
-    <row r="66" spans="1:5">
+      <c r="D65" s="9"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="4"/>
+    </row>
+    <row r="66" spans="1:8">
       <c r="A66" s="1" t="s">
         <v>158</v>
       </c>
@@ -2371,12 +2513,15 @@
       <c r="C66" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D66" s="5" t="s">
+      <c r="D66" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="E66" s="8"/>
-    </row>
-    <row r="67" spans="1:5">
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="4"/>
+    </row>
+    <row r="67" spans="1:8">
       <c r="A67" s="1" t="s">
         <v>160</v>
       </c>
@@ -2386,12 +2531,15 @@
       <c r="C67" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D67" s="5" t="s">
+      <c r="D67" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="E67" s="8"/>
-    </row>
-    <row r="68" spans="1:5">
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="4"/>
+    </row>
+    <row r="68" spans="1:8">
       <c r="A68" s="1" t="s">
         <v>162</v>
       </c>
@@ -2401,10 +2549,13 @@
       <c r="C68" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D68" s="5"/>
-      <c r="E68" s="8"/>
-    </row>
-    <row r="69" spans="1:5">
+      <c r="D68" s="9"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="4"/>
+    </row>
+    <row r="69" spans="1:8">
       <c r="A69" s="1" t="s">
         <v>164</v>
       </c>
@@ -2414,12 +2565,15 @@
       <c r="C69" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D69" s="5" t="s">
+      <c r="D69" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="E69" s="8"/>
-    </row>
-    <row r="70" spans="1:5">
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="4"/>
+    </row>
+    <row r="70" spans="1:8">
       <c r="A70" s="1" t="s">
         <v>166</v>
       </c>
@@ -2429,10 +2583,13 @@
       <c r="C70" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D70" s="5"/>
-      <c r="E70" s="8"/>
-    </row>
-    <row r="71" spans="1:5">
+      <c r="D70" s="9"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="4"/>
+    </row>
+    <row r="71" spans="1:8">
       <c r="A71" s="1" t="s">
         <v>168</v>
       </c>
@@ -2442,10 +2599,13 @@
       <c r="C71" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D71" s="5"/>
-      <c r="E71" s="8"/>
-    </row>
-    <row r="72" spans="1:5">
+      <c r="D71" s="9"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
+      <c r="G71" s="5"/>
+      <c r="H71" s="4"/>
+    </row>
+    <row r="72" spans="1:8">
       <c r="A72" s="1" t="s">
         <v>170</v>
       </c>
@@ -2455,12 +2615,15 @@
       <c r="C72" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D72" s="5" t="s">
+      <c r="D72" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="E72" s="8"/>
-    </row>
-    <row r="73" spans="1:5">
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
+      <c r="G72" s="5"/>
+      <c r="H72" s="4"/>
+    </row>
+    <row r="73" spans="1:8">
       <c r="A73" s="1" t="s">
         <v>173</v>
       </c>
@@ -2470,10 +2633,13 @@
       <c r="C73" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D73" s="5"/>
-      <c r="E73" s="8"/>
-    </row>
-    <row r="74" spans="1:5">
+      <c r="D73" s="9"/>
+      <c r="E73" s="5"/>
+      <c r="F73" s="5"/>
+      <c r="G73" s="5"/>
+      <c r="H73" s="4"/>
+    </row>
+    <row r="74" spans="1:8">
       <c r="A74" s="1" t="s">
         <v>175</v>
       </c>
@@ -2483,10 +2649,13 @@
       <c r="C74" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D74" s="5"/>
-      <c r="E74" s="8"/>
-    </row>
-    <row r="75" spans="1:5">
+      <c r="D74" s="9"/>
+      <c r="E74" s="5"/>
+      <c r="F74" s="5"/>
+      <c r="G74" s="5"/>
+      <c r="H74" s="4"/>
+    </row>
+    <row r="75" spans="1:8">
       <c r="A75" s="1" t="s">
         <v>177</v>
       </c>
@@ -2496,12 +2665,15 @@
       <c r="C75" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="D75" s="5" t="s">
+      <c r="D75" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="E75" s="8"/>
-    </row>
-    <row r="76" spans="1:5">
+      <c r="E75" s="5"/>
+      <c r="F75" s="5"/>
+      <c r="G75" s="5"/>
+      <c r="H75" s="4"/>
+    </row>
+    <row r="76" spans="1:8">
       <c r="A76" s="1" t="s">
         <v>180</v>
       </c>
@@ -2511,10 +2683,13 @@
       <c r="C76" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="D76" s="5"/>
-      <c r="E76" s="8"/>
-    </row>
-    <row r="77" spans="1:5">
+      <c r="D76" s="9"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="5"/>
+      <c r="G76" s="5"/>
+      <c r="H76" s="4"/>
+    </row>
+    <row r="77" spans="1:8">
       <c r="A77" s="1" t="s">
         <v>183</v>
       </c>
@@ -2524,10 +2699,13 @@
       <c r="C77" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="D77" s="5"/>
-      <c r="E77" s="8"/>
-    </row>
-    <row r="78" spans="1:5">
+      <c r="D77" s="9"/>
+      <c r="E77" s="5"/>
+      <c r="F77" s="5"/>
+      <c r="G77" s="5"/>
+      <c r="H77" s="4"/>
+    </row>
+    <row r="78" spans="1:8">
       <c r="A78" s="1" t="s">
         <v>185</v>
       </c>
@@ -2537,12 +2715,15 @@
       <c r="C78" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="D78" s="5" t="s">
+      <c r="D78" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="E78" s="8"/>
-    </row>
-    <row r="79" spans="1:5">
+      <c r="E78" s="5"/>
+      <c r="F78" s="5"/>
+      <c r="G78" s="5"/>
+      <c r="H78" s="4"/>
+    </row>
+    <row r="79" spans="1:8">
       <c r="A79" s="1" t="s">
         <v>188</v>
       </c>
@@ -2552,12 +2733,15 @@
       <c r="C79" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="D79" s="5" t="s">
+      <c r="D79" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="E79" s="8"/>
-    </row>
-    <row r="80" spans="1:5">
+      <c r="E79" s="5"/>
+      <c r="F79" s="5"/>
+      <c r="G79" s="5"/>
+      <c r="H79" s="4"/>
+    </row>
+    <row r="80" spans="1:8">
       <c r="A80" s="1" t="s">
         <v>191</v>
       </c>
@@ -2567,67 +2751,103 @@
       <c r="C80" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="D80" s="5" t="s">
+      <c r="D80" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="E80" s="8"/>
-    </row>
-    <row r="81" spans="5:5">
-      <c r="E81" s="7"/>
-    </row>
-    <row r="82" spans="5:5">
-      <c r="E82" s="7"/>
-    </row>
-    <row r="83" spans="5:5">
-      <c r="E83" s="7"/>
-    </row>
-    <row r="84" spans="5:5">
-      <c r="E84" s="7"/>
-    </row>
-    <row r="85" spans="5:5">
-      <c r="E85" s="7"/>
-    </row>
-    <row r="86" spans="5:5">
-      <c r="E86" s="7"/>
-    </row>
-    <row r="87" spans="5:5">
-      <c r="E87" s="7"/>
-    </row>
-    <row r="88" spans="5:5">
-      <c r="E88" s="7"/>
-    </row>
-    <row r="89" spans="5:5">
-      <c r="E89" s="7"/>
-    </row>
-    <row r="90" spans="5:5">
-      <c r="E90" s="7"/>
-    </row>
-    <row r="91" spans="5:5">
-      <c r="E91" s="7"/>
-    </row>
-    <row r="92" spans="5:5">
-      <c r="E92" s="7"/>
-    </row>
-    <row r="93" spans="5:5">
-      <c r="E93" s="7"/>
-    </row>
-    <row r="94" spans="5:5">
-      <c r="E94" s="7"/>
-    </row>
-    <row r="95" spans="5:5">
-      <c r="E95" s="7"/>
-    </row>
-    <row r="96" spans="5:5">
-      <c r="E96" s="7"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="5"/>
+      <c r="G80" s="5"/>
+      <c r="H80" s="4"/>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D81" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="E81" s="5"/>
+      <c r="F81" s="5"/>
+      <c r="G81" s="5"/>
+      <c r="H81" s="4"/>
+    </row>
+    <row r="82" spans="1:8">
+      <c r="A82" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D82" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="E82" s="4"/>
+      <c r="F82" s="4"/>
+      <c r="G82" s="4"/>
+      <c r="H82" s="4"/>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="E83" s="4"/>
+      <c r="F83" s="4"/>
+      <c r="G83" s="4"/>
+      <c r="H83" s="4"/>
+    </row>
+    <row r="84" spans="1:8">
+      <c r="E84" s="4"/>
+      <c r="F84" s="4"/>
+      <c r="G84" s="4"/>
+      <c r="H84" s="4"/>
+    </row>
+    <row r="85" spans="1:8">
+      <c r="E85" s="4"/>
+    </row>
+    <row r="86" spans="1:8">
+      <c r="E86" s="4"/>
+    </row>
+    <row r="87" spans="1:8">
+      <c r="E87" s="4"/>
+    </row>
+    <row r="88" spans="1:8">
+      <c r="E88" s="4"/>
+    </row>
+    <row r="89" spans="1:8">
+      <c r="E89" s="4"/>
+    </row>
+    <row r="90" spans="1:8">
+      <c r="E90" s="4"/>
+    </row>
+    <row r="91" spans="1:8">
+      <c r="E91" s="4"/>
+    </row>
+    <row r="92" spans="1:8">
+      <c r="E92" s="4"/>
+    </row>
+    <row r="93" spans="1:8">
+      <c r="E93" s="4"/>
+    </row>
+    <row r="94" spans="1:8">
+      <c r="E94" s="4"/>
+    </row>
+    <row r="95" spans="1:8">
+      <c r="E95" s="4"/>
+    </row>
+    <row r="96" spans="1:8">
+      <c r="E96" s="4"/>
     </row>
     <row r="97" spans="5:5">
-      <c r="E97" s="7"/>
+      <c r="E97" s="4"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D12" r:id="rId1" display="https://lcsc.com/product-detail/DC-DC-Converters_Texas-Instruments-TPS54335ADRCR_C473400.html" xr:uid="{B63F5762-D0C9-4360-9000-6F08D92680C9}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>